<commit_message>
[imp] update menu order
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/devops_service/hzero_platform/hzero-menu-user-role-label.xlsx
+++ b/src/main/resources/script/db/init-data/devops_service/hzero_platform/hzero-menu-user-role-label.xlsx
@@ -8740,9 +8740,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="67">
@@ -8989,6 +8989,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -9003,10 +9019,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9018,25 +9035,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9055,18 +9072,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9094,14 +9119,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
@@ -9110,31 +9127,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9216,7 +9216,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9228,13 +9258,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9246,85 +9306,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9342,7 +9336,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9354,49 +9384,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9518,6 +9518,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -9533,6 +9553,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -9544,33 +9573,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9592,159 +9594,157 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="24" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="33" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="33" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="52" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="47" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -10485,8 +10485,8 @@
   <sheetPr/>
   <dimension ref="A1:X200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="F201" sqref="F201"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" topLeftCell="F167" workbookViewId="0">
+      <selection activeCell="L202" sqref="L202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
@@ -19486,6 +19486,9 @@
       </c>
       <c r="L199" t="s">
         <v>87</v>
+      </c>
+      <c r="M199">
+        <v>80</v>
       </c>
       <c r="N199">
         <v>1</v>

</xml_diff>